<commit_message>
modified Dashboard Main.vi and added some overrides
</commit_message>
<xml_diff>
--- a/ king-kong-2230-2013/Documents/data sending.xlsx
+++ b/ king-kong-2230-2013/Documents/data sending.xlsx
@@ -184,10 +184,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -506,19 +506,19 @@
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="19.125" customWidth="1"/>
-    <col min="3" max="3" width="1.625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="1.625" style="2" customWidth="1"/>
     <col min="5" max="5" width="16.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="D1" s="2" t="s">
+      <c r="B1" s="3"/>
+      <c r="D1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="2"/>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
@@ -641,16 +641,16 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="3" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:5" s="2" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="D15" s="2" t="s">
+      <c r="B15" s="3"/>
+      <c r="D15" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="2"/>
+      <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">

</xml_diff>